<commit_message>
Añado excepciones y 5 digitos de entrada referencia
</commit_message>
<xml_diff>
--- a/Repuestos2024.xlsx
+++ b/Repuestos2024.xlsx
@@ -1,87 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16729"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fly_c\Desktop\Proyecto1\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7410"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7410" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
-  <si>
-    <t>Ref.Componente</t>
-  </si>
-  <si>
-    <t>Frontal</t>
-  </si>
-  <si>
-    <t>Lateral Der.</t>
-  </si>
-  <si>
-    <t>Lateral Izq.</t>
-  </si>
-  <si>
-    <t>Power/Reset</t>
-  </si>
-  <si>
-    <t>Leds frontales</t>
-  </si>
-  <si>
-    <t>Varios</t>
-  </si>
-  <si>
-    <t>Protecciones</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -100,22 +46,81 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -403,74 +408,212 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="14" style="1" customWidth="1"/>
+    <col width="18" customWidth="1" style="1" min="1" max="1"/>
+    <col width="12.42578125" customWidth="1" style="1" min="3" max="3"/>
+    <col width="11.42578125" customWidth="1" style="1" min="4" max="4"/>
+    <col width="14.5703125" customWidth="1" style="1" min="5" max="5"/>
+    <col width="12.85546875" customWidth="1" style="1" min="6" max="6"/>
+    <col width="14" customWidth="1" style="1" min="8" max="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Ref.Componente</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Frontal</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Lateral Der.</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Lateral Izq.</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Power/Reset</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Leds frontales</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Varios</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Protecciones</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" t="s">
-        <v>9</v>
-      </c>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>ventilador</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Pruebas con ref de 5 digitos
</commit_message>
<xml_diff>
--- a/Repuestos2024.xlsx
+++ b/Repuestos2024.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
@@ -603,17 +603,95 @@
           <t>10</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr"/>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr">
         <is>
           <t>ventilador</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>11111</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>11112</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>ventilador, chapa trasera</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Ahora tras guardar o buscar limpia el formulario salvo la ref
</commit_message>
<xml_diff>
--- a/Repuestos2024.xlsx
+++ b/Repuestos2024.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
@@ -693,6 +693,32 @@
         </is>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>11113</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>flaikers</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Elimino ejecutable,retoque comentarios,desactiva formulario
</commit_message>
<xml_diff>
--- a/Repuestos2024.xlsx
+++ b/Repuestos2024.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
@@ -630,11 +630,7 @@
           <t>3</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
+      <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr">
         <is>
           <t>5</t>
@@ -642,7 +638,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>no pero si</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -704,20 +700,75 @@
           <t>1</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
       <c r="G8" t="inlineStr">
         <is>
           <t>flaikers</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>67555</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>12345</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>COSINES</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Correcciones de avisos, Intro para busqueda y desactiva formulario (#2), Nombre en titulo, retoque en comentarios.
* Corregidos los 6 por 5 añado ejecutable

* Cambio el nombre a INVOLUCRO 2000 y ajusto ventana

* Pulsa intro y hace la busqueda

* Elimino ejecutable,retoque comentarios,desactiva formulario
</commit_message>
<xml_diff>
--- a/Repuestos2024.xlsx
+++ b/Repuestos2024.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
@@ -630,11 +630,7 @@
           <t>3</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
+      <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr">
         <is>
           <t>5</t>
@@ -642,7 +638,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>no pero si</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -704,20 +700,75 @@
           <t>1</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
       <c r="G8" t="inlineStr">
         <is>
           <t>flaikers</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>67555</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>12345</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>COSINES</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Añado funcion para que bloquee Guardar al escribir nueva ref
</commit_message>
<xml_diff>
--- a/Repuestos2024.xlsx
+++ b/Repuestos2024.xlsx
@@ -630,7 +630,6 @@
           <t>3</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr">
         <is>
           <t>5</t>
@@ -700,14 +699,30 @@
           <t>1</t>
         </is>
       </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="D8" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>flaikers</t>
+          <t>no pero si</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -746,12 +761,12 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -761,7 +776,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>COSINES</t>
+          <t>no pero si</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">

</xml_diff>

<commit_message>
Bloqueo Guardar y Ejecutable (#3)
* Añado funcion para que bloquee Guardar al escribir nueva ref

* Añado ejecutable con carpetas
</commit_message>
<xml_diff>
--- a/Repuestos2024.xlsx
+++ b/Repuestos2024.xlsx
@@ -630,7 +630,6 @@
           <t>3</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr">
         <is>
           <t>5</t>
@@ -700,14 +699,30 @@
           <t>1</t>
         </is>
       </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="D8" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>flaikers</t>
+          <t>no pero si</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -746,12 +761,12 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -761,7 +776,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>COSINES</t>
+          <t>no pero si</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">

</xml_diff>